<commit_message>
Improved code on batman
</commit_message>
<xml_diff>
--- a/batman defuses bomb/batman difuses bomb diagram.xlsx
+++ b/batman defuses bomb/batman difuses bomb diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Menelik Tefera\Documents\Personal\algorithms\batman defuses bomb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8CB89C-CD4F-4EE7-BEEB-B3299E28C9C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E59D03A-E48D-4B83-83C5-4BA7ECCC4E89}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9339077A-B857-4FCE-B3A0-619E784266E2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>B</t>
   </si>
@@ -44,91 +44,20 @@
     <t>max</t>
   </si>
   <si>
-    <t>[ 6, 3 ]</t>
+    <t>first move to [ 6, 3 ]</t>
   </si>
   <si>
-    <t>[ 8, 1 ]</t>
+    <t>Second move to [ 8, 1 ]</t>
   </si>
   <si>
-    <t>[ 8, 2 ]</t>
-  </si>
-  <si>
-    <t>[ 7, 2 ]</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>min</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>max</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>min</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>max</t>
-    </r>
+    <t>Final move to [ 7, 2 ]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,13 +90,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="28"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -229,15 +151,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="26"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +177,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,11 +226,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -307,51 +237,78 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="1" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="1" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -667,251 +624,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A392D87D-B3A2-4711-8D7A-9305FD695C83}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" style="4" customWidth="1"/>
     <col min="2" max="12" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="L1" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2">
+        <v>6</v>
+      </c>
+      <c r="J2" s="5">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2">
         <v>8</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L2" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+    </row>
+    <row r="4" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="25"/>
+      <c r="M4" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A5" s="10"/>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="26"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="24"/>
+    </row>
+    <row r="6" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3">
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="B7" s="3">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="19"/>
+    </row>
+    <row r="8" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="3">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+    </row>
+    <row r="9" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="9"/>
+      <c r="B9" s="3">
+        <v>6</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+    </row>
+    <row r="10" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="B10" s="3">
+        <v>7</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="3">
+        <v>8</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3">
-        <v>4</v>
-      </c>
-      <c r="H2" s="3">
-        <v>5</v>
-      </c>
-      <c r="I2" s="3">
-        <v>6</v>
-      </c>
-      <c r="J2" s="8">
-        <v>7</v>
-      </c>
-      <c r="K2" s="3">
-        <v>8</v>
-      </c>
-      <c r="L2" s="3">
+      <c r="B12" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="6"/>
-      <c r="K4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A5" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="4">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="B7" s="4">
-        <v>4</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="4">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="4">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="B10" s="4">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="4">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="4">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I14" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="12"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>